<commit_message>
adding validation for authentication
</commit_message>
<xml_diff>
--- a/public/excel/datalaporan (1).xlsx
+++ b/public/excel/datalaporan (1).xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9924"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="279">
   <si>
     <t>Nama</t>
   </si>
@@ -85,7 +86,7 @@
     <t>kuliah</t>
   </si>
   <si>
-    <t>01/01/2003</t>
+    <t>2003/01/01</t>
   </si>
   <si>
     <t>laki-laki</t>
@@ -124,7 +125,7 @@
     <t>kerja</t>
   </si>
   <si>
-    <t>02/02/2004</t>
+    <t>2004/02/02</t>
   </si>
   <si>
     <t>perempuan</t>
@@ -157,7 +158,7 @@
     <t>menganggur</t>
   </si>
   <si>
-    <t>03/03/2005</t>
+    <t>2005/03/03</t>
   </si>
   <si>
     <t>Dedi Prasetyo</t>
@@ -181,7 +182,7 @@
     <t>Yogyakarta</t>
   </si>
   <si>
-    <t>04/04/2006</t>
+    <t>2006/04/04</t>
   </si>
   <si>
     <t>Universitas Gadjah Mada</t>
@@ -202,7 +203,7 @@
     <t>dwisetiawan@yahoo.com</t>
   </si>
   <si>
-    <t>05/05/2007</t>
+    <t>2007/05/05</t>
   </si>
   <si>
     <t>PT Tekno Bersama</t>
@@ -223,7 +224,7 @@
     <t>rinawulandari@gmail.com</t>
   </si>
   <si>
-    <t>06/06/2008</t>
+    <t>2008/06/06</t>
   </si>
   <si>
     <t>Universitas Padjajaran</t>
@@ -244,7 +245,7 @@
     <t>hendrasantoso@yahoo.com</t>
   </si>
   <si>
-    <t>07/07/2009</t>
+    <t>2009/07/07</t>
   </si>
   <si>
     <t>PT Sehat Bersama</t>
@@ -271,7 +272,7 @@
     <t>Denpasar</t>
   </si>
   <si>
-    <t>08/08/2010</t>
+    <t>2010/08/08</t>
   </si>
   <si>
     <t>Irfan Susanto</t>
@@ -289,7 +290,7 @@
     <t>aldicahyono@gmail.com</t>
   </si>
   <si>
-    <t>09/09/2011</t>
+    <t>2011/09/09</t>
   </si>
   <si>
     <t>Joko Widodo</t>
@@ -307,7 +308,7 @@
     <t>dinapermata@yahoo.com</t>
   </si>
   <si>
-    <t>10/10/2012</t>
+    <t>2012/10/10</t>
   </si>
   <si>
     <t>Kurniawan Santoso</t>
@@ -322,7 +323,7 @@
     <t>yogapradana@outlook.com</t>
   </si>
   <si>
-    <t>11/11/2013</t>
+    <t>2013/11/11</t>
   </si>
   <si>
     <t>Luthfi Abdul</t>
@@ -340,7 +341,7 @@
     <t>sitinurhayati@gmail.com</t>
   </si>
   <si>
-    <t>12/12/2014</t>
+    <t>2014/12/12</t>
   </si>
   <si>
     <t>Miftahul Huda</t>
@@ -358,7 +359,7 @@
     <t>bambangkurniawan@yahoo.com</t>
   </si>
   <si>
-    <t>01/13/2015</t>
+    <t>2015/01/13</t>
   </si>
   <si>
     <t>Nanda Pratama</t>
@@ -376,7 +377,7 @@
     <t>sitiwulandari@gmail.com</t>
   </si>
   <si>
-    <t>02/14/2016</t>
+    <t>2016/02/14</t>
   </si>
   <si>
     <t>Oktavianus Setiawan</t>
@@ -394,7 +395,7 @@
     <t>hendrapratama@outlook.com</t>
   </si>
   <si>
-    <t>03/15/2017</t>
+    <t>2017/03/15</t>
   </si>
   <si>
     <t>Prasetyo Wibowo</t>
@@ -412,7 +413,7 @@
     <t>ritadevi@yahoo.com</t>
   </si>
   <si>
-    <t>04/16/2018</t>
+    <t>2018/04/16</t>
   </si>
   <si>
     <t>Qori Rusdianto</t>
@@ -430,7 +431,7 @@
     <t>diannugraha@gmail.com</t>
   </si>
   <si>
-    <t>05/17/2019</t>
+    <t>2019/05/17</t>
   </si>
   <si>
     <t>Universitas Airlangga</t>
@@ -451,7 +452,7 @@
     <t>sitirahmawati@outlook.com</t>
   </si>
   <si>
-    <t>06/18/2020</t>
+    <t>2020/06/18</t>
   </si>
   <si>
     <t>Slamet Santoso</t>
@@ -469,7 +470,7 @@
     <t>riansuryanto@gmail.com</t>
   </si>
   <si>
-    <t>07/19/2021</t>
+    <t>2021/07/19</t>
   </si>
   <si>
     <t>Teguh Wijaya</t>
@@ -487,7 +488,7 @@
     <t>rinadewi@yahoo.com</t>
   </si>
   <si>
-    <t>08/20/2022</t>
+    <t>2022/08/20</t>
   </si>
   <si>
     <t>Umar Abdullah</t>
@@ -505,7 +506,7 @@
     <t>fajarramadhan@outlook.com</t>
   </si>
   <si>
-    <t>09/21/2023</t>
+    <t>2023/09/21</t>
   </si>
   <si>
     <t>Vicky Prasetyo</t>
@@ -523,7 +524,7 @@
     <t>dewiayu@gmail.com</t>
   </si>
   <si>
-    <t>10/22/2024</t>
+    <t>2024/10/22</t>
   </si>
   <si>
     <t>Wahyu Nugroho</t>
@@ -541,7 +542,7 @@
     <t>hendrawijaya@yahoo.com</t>
   </si>
   <si>
-    <t>11/23/2025</t>
+    <t>2025/11/23</t>
   </si>
   <si>
     <t>Xavier Alimudin</t>
@@ -559,7 +560,7 @@
     <t>ritasusanti@outlook.com</t>
   </si>
   <si>
-    <t>12/24/2026</t>
+    <t>2026/12/24</t>
   </si>
   <si>
     <t>Yanto Susanto</t>
@@ -574,7 +575,7 @@
     <t>budisantoso@gmail.com</t>
   </si>
   <si>
-    <t>01/25/2027</t>
+    <t>2027/01/25</t>
   </si>
   <si>
     <t>Zainul Arifin</t>
@@ -592,7 +593,7 @@
     <t>sitirahayu@yahoo.com</t>
   </si>
   <si>
-    <t>02/26/2028</t>
+    <t>2028/02/26</t>
   </si>
   <si>
     <t>Abdul Hakim</t>
@@ -610,7 +611,7 @@
     <t>andiprabowo@outlook.com</t>
   </si>
   <si>
-    <t>03/27/2029</t>
+    <t>2029/03/27</t>
   </si>
   <si>
     <t>Basuki Wibowo</t>
@@ -628,7 +629,7 @@
     <t>dininuraini@gmail.com</t>
   </si>
   <si>
-    <t>04/28/2030</t>
+    <t>2030/04/28</t>
   </si>
   <si>
     <t>Cahyo Nugroho</t>
@@ -643,7 +644,7 @@
     <t>riansuryanto@yahoo.com</t>
   </si>
   <si>
-    <t>05/29/2031</t>
+    <t>2031/05/29</t>
   </si>
   <si>
     <t>Denny Prasetyo</t>
@@ -658,7 +659,7 @@
     <t>sitiwulandari@outlook.com</t>
   </si>
   <si>
-    <t>06/30/2032</t>
+    <t>2032/06/30</t>
   </si>
   <si>
     <t>Edy Suryanto</t>
@@ -673,7 +674,7 @@
     <t>hendrapratama@gmail.com</t>
   </si>
   <si>
-    <t>07/31/2033</t>
+    <t>2033/07/31</t>
   </si>
   <si>
     <t>Fahrul Rahman</t>
@@ -685,7 +686,7 @@
     <t>pelayan hotel</t>
   </si>
   <si>
-    <t>08/30/2034</t>
+    <t>2034/08/30</t>
   </si>
   <si>
     <t>Gilang Pratama</t>
@@ -700,7 +701,7 @@
     <t>diannugraha@outlook.com</t>
   </si>
   <si>
-    <t>09/30/2035</t>
+    <t>2035/09/30</t>
   </si>
   <si>
     <t>Gita Rahayu</t>
@@ -712,7 +713,7 @@
     <t>sitirahmawati@gmail.com</t>
   </si>
   <si>
-    <t>10/30/2036</t>
+    <t>2036/10/30</t>
   </si>
   <si>
     <t>Iwan Santoso</t>
@@ -724,7 +725,7 @@
     <t>pengacara</t>
   </si>
   <si>
-    <t>11/30/2037</t>
+    <t>2037/11/30</t>
   </si>
   <si>
     <t>Joko Nugroho</t>
@@ -739,7 +740,7 @@
     <t>rinadewi@outlook.com</t>
   </si>
   <si>
-    <t>12/30/2038</t>
+    <t>2038/12/30</t>
   </si>
   <si>
     <t>Kusumo Wibowo</t>
@@ -754,7 +755,7 @@
     <t>fajarramadhan@gmail.com</t>
   </si>
   <si>
-    <t>01/30/2039</t>
+    <t>2039/01/30</t>
   </si>
   <si>
     <t>Lukman Hakim</t>
@@ -769,7 +770,7 @@
     <t>dewiayu@yahoo.com</t>
   </si>
   <si>
-    <t>02/28/2040</t>
+    <t>2040/02/28</t>
   </si>
   <si>
     <t>Muharrom Wijaya</t>
@@ -781,7 +782,7 @@
     <t>hendrawijaya@outlook.com</t>
   </si>
   <si>
-    <t>03/24/2041</t>
+    <t>2041/03/24</t>
   </si>
   <si>
     <t>Nizar Abdullah</t>
@@ -796,7 +797,7 @@
     <t>ritasusanti@gmail.com</t>
   </si>
   <si>
-    <t>04/23/2042</t>
+    <t>2042/04/23</t>
   </si>
   <si>
     <t>Oka Prasetyo</t>
@@ -808,7 +809,7 @@
     <t>budisantoso@outlook.com</t>
   </si>
   <si>
-    <t>05/24/2043</t>
+    <t>2043/05/24</t>
   </si>
   <si>
     <t>Prayoga Wicaksono</t>
@@ -817,7 +818,7 @@
     <t>manajer proyek</t>
   </si>
   <si>
-    <t>06/21/2044</t>
+    <t>2044/06/21</t>
   </si>
   <si>
     <t>Qori Rusman</t>
@@ -832,7 +833,7 @@
     <t>andiprabowo@gmail.com</t>
   </si>
   <si>
-    <t>07/25/2045</t>
+    <t>2045/07/25</t>
   </si>
   <si>
     <t>Rahmat Santoso</t>
@@ -844,7 +845,7 @@
     <t>dininuraini@outlook.com</t>
   </si>
   <si>
-    <t>08/26/2046</t>
+    <t>2046/08/26</t>
   </si>
   <si>
     <t>Sigit Wibowo</t>
@@ -856,367 +857,28 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="21">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1224,315 +886,21 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <dxfs count="0"/>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -1817,37 +1185,41 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="21.1388888888889" customWidth="1"/>
-    <col min="2" max="2" width="34.1388888888889" customWidth="1"/>
-    <col min="3" max="3" width="31.7037037037037" customWidth="1"/>
-    <col min="4" max="5" width="12.8518518518519" customWidth="1"/>
-    <col min="6" max="6" width="10.5648148148148" customWidth="1"/>
-    <col min="7" max="7" width="12.8518518518519" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="15.2777777777778" customWidth="1"/>
-    <col min="10" max="10" width="16.4259259259259" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.4259259259259" customWidth="1"/>
-    <col min="12" max="12" width="21.1388888888889" customWidth="1"/>
-    <col min="13" max="13" width="19.9907407407407" customWidth="1"/>
-    <col min="14" max="14" width="28.1388888888889" customWidth="1"/>
-    <col min="15" max="15" width="23.4259259259259" customWidth="1"/>
-    <col min="16" max="16" width="25.8518518518519" customWidth="1"/>
-    <col min="17" max="17" width="18.712962962963" customWidth="1"/>
-    <col min="18" max="18" width="24.7037037037037" customWidth="1"/>
+    <col min="1" max="1" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="34.135" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="31.707" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="12.854" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="12.854" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="10.569" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="12.854" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="13.997" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="15.282" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="16.425" bestFit="true" customWidth="true" style="1"/>
+    <col min="11" max="11" width="16.425" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="19.995" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="28.136" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="23.423" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="25.851" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="18.71" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="24.708" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -4206,8 +3578,17 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>